<commit_message>
Add a custom date to a custom style in examples.xlsx
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="124">
   <si>
     <t>normal</t>
   </si>
@@ -624,15 +624,19 @@
   <si>
     <t>Cell merged into cell below</t>
   </si>
+  <si>
+    <t>custom style with custom date format</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-1409]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\ mmmm\ dddd"/>
     <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1214,13 +1218,13 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1242,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -1290,8 +1294,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
@@ -1300,18 +1304,18 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1321,7 +1325,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="stylealign" xfId="2"/>
+    <cellStyle name="styledate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1390,11 +1394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129909120"/>
-        <c:axId val="129910656"/>
+        <c:axId val="132530560"/>
+        <c:axId val="132532096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129909120"/>
+        <c:axId val="132530560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129910656"/>
+        <c:crossAx val="132532096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129910656"/>
+        <c:axId val="132532096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129909120"/>
+        <c:crossAx val="132530560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1786,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2069,437 +2073,445 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="13">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+    <row r="40" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55" t="s">
+    <row r="41" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="75" t="s">
+    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="75"/>
-    </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="75"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="72" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="73" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="20" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="67" t="s">
-        <v>62</v>
+      <c r="B52" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B53" s="68" t="s">
-        <v>63</v>
+      <c r="B53" s="67" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="69" t="s">
+      <c r="B54" s="68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="57" t="s">
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B56" s="66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B57" s="70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="70" t="s">
+      <c r="B58" s="70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="70" t="s">
+      <c r="B59" s="70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="45" t="s">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="70" t="s">
+      <c r="B60" s="70" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="70" t="s">
+      <c r="B61" s="70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="47" t="s">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B62" s="70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="48" t="s">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="70" t="s">
+      <c r="B63" s="70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="70" t="s">
+      <c r="B64" s="70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="50" t="s">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="70" t="s">
+      <c r="B65" s="70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="51" t="s">
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B66" s="70" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="52" t="s">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="70" t="s">
+      <c r="B67" s="70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="53" t="s">
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="70" t="s">
+      <c r="B68" s="70" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
-      <c r="B68" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="40"/>
+      <c r="B69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="22"/>
-      <c r="B69" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="22"/>
+      <c r="B70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="23"/>
-      <c r="B70" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="23"/>
+      <c r="B71" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="24"/>
+      <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="25"/>
+      <c r="B73" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="26"/>
-      <c r="B73" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="26"/>
+      <c r="B74" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="27"/>
-      <c r="B74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="27"/>
+      <c r="B75" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="28"/>
-      <c r="B75" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="28"/>
+      <c r="B76" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
-      <c r="B76" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="29"/>
+      <c r="B77" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="30"/>
+      <c r="B78" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="31"/>
-      <c r="B78" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="31"/>
+      <c r="B79" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="32"/>
-      <c r="B79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="32"/>
+      <c r="B80" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="33"/>
-      <c r="B80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="33"/>
+      <c r="B81" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="34"/>
-      <c r="B81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="34"/>
+      <c r="B82" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="35"/>
-      <c r="B82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="35"/>
+      <c r="B83" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="B83" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="36"/>
+      <c r="B84" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="37"/>
+      <c r="B85" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="38"/>
-      <c r="B85" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="38"/>
+      <c r="B86" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="39"/>
-      <c r="B86" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="39"/>
+      <c r="B87" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="58"/>
-      <c r="B87" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="58"/>
+      <c r="B88" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="59"/>
-      <c r="B88" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="59"/>
+      <c r="B89" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="60"/>
-      <c r="B89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="60"/>
+      <c r="B90" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="61"/>
-      <c r="B90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="62"/>
-      <c r="B91" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="63"/>
-      <c r="B92" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="63"/>
+      <c r="B93" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A65" r:id="rId1"/>
-    <hyperlink ref="A66" r:id="rId2"/>
+    <hyperlink ref="A66" r:id="rId1"/>
+    <hyperlink ref="A67" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Warn when dates have the Excel off-by-one bug
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -1394,11 +1394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132530560"/>
-        <c:axId val="132532096"/>
+        <c:axId val="144213504"/>
+        <c:axId val="144226560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132530560"/>
+        <c:axId val="144213504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132532096"/>
+        <c:crossAx val="144226560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1415,7 +1415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132532096"/>
+        <c:axId val="144226560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,7 +1426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132530560"/>
+        <c:crossAx val="144213504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1793,7 +1793,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Add test for unicode string ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
   <si>
     <t>normal</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>custom style with custom date format</t>
+  </si>
+  <si>
+    <t>unicode shrug</t>
+  </si>
+  <si>
+    <t>¯\_(ツ)_/¯</t>
   </si>
 </sst>
 </file>
@@ -1790,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2503,6 +2509,14 @@
       <c r="A93" s="63"/>
       <c r="B93" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>125</v>
+      </c>
+      <c r="B94" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't detect 'd' in '[Red]' in number formats as date
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="127">
   <si>
     <t>normal</t>
   </si>
@@ -633,16 +633,20 @@
   <si>
     <t>¯\_(ツ)_/¯</t>
   </si>
+  <si>
+    <t>custom number format with 'd' in [Red] to confuse date detection heuristic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-1409]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\ mmmm\ dddd"/>
     <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1232,7 +1236,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1324,6 +1328,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1400,11 +1405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144213504"/>
-        <c:axId val="144226560"/>
+        <c:axId val="144227712"/>
+        <c:axId val="144843904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144213504"/>
+        <c:axId val="144227712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144226560"/>
+        <c:crossAx val="144843904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144226560"/>
+        <c:axId val="144843904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144213504"/>
+        <c:crossAx val="144227712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1796,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:B94"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2517,6 +2522,14 @@
       </c>
       <c r="B94" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="76">
+        <v>-1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Return underline as NA when none present
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -858,7 +858,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -1186,6 +1186,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1512,7 +1518,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1607,6 +1613,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1683,11 +1690,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128595840"/>
-        <c:axId val="128597376"/>
+        <c:axId val="133673728"/>
+        <c:axId val="133675264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128595840"/>
+        <c:axId val="133673728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128597376"/>
+        <c:crossAx val="133675264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1704,7 +1711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128597376"/>
+        <c:axId val="133675264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128595840"/>
+        <c:crossAx val="133673728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2081,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2337,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="79" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">

</xml_diff>

<commit_message>
Test numFmts and fonts
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="160">
   <si>
     <t>normal</t>
   </si>
@@ -846,6 +846,24 @@
       <t xml:space="preserve"> with cell-level defaults</t>
     </r>
   </si>
+  <si>
+    <t>underline single accounting</t>
+  </si>
+  <si>
+    <t>underline double accounting</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>tint</t>
+  </si>
 </sst>
 </file>
 
@@ -858,7 +876,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -1192,6 +1210,42 @@
     <font>
       <u/>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="doubleAccounting"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1518,7 +1572,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1610,10 +1664,16 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1690,11 +1750,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133673728"/>
-        <c:axId val="133675264"/>
+        <c:axId val="125910016"/>
+        <c:axId val="128404864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133673728"/>
+        <c:axId val="125910016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133675264"/>
+        <c:crossAx val="128404864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1711,7 +1771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133675264"/>
+        <c:axId val="128404864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,7 +1782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133673728"/>
+        <c:crossAx val="125910016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2086,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2337,7 +2397,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="78" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
@@ -2441,7 +2501,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="79" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2449,7 +2509,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="78"/>
+      <c r="A43" s="79"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3083,11 +3143,59 @@
         <v>152</v>
       </c>
     </row>
+    <row r="133" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B133" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="B134" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="82" t="s">
+        <v>156</v>
+      </c>
+      <c r="B135" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A136" s="83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B136" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A137" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="B137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="B138" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A42:A43"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations disablePrompts="1" count="15">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error title" error="error body" promptTitle="message title" prompt="message body" sqref="A106">
       <formula1>0</formula1>
       <formula2>9</formula2>

</xml_diff>

<commit_message>
Refactor gradientFill to expose 'stops'
'Stops' define the extremes of each gradient, their colour, and where in the
cell they occur.
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -11,9 +11,10 @@
     <sheet name="1~`!@#$%^&amp;()_-+={}|;&quot;'&lt;,&gt;.£¹÷¦°" sheetId="2" r:id="rId2"/>
     <sheet name="chart-not-imported" sheetId="4" r:id="rId3"/>
     <sheet name="E09904.2" sheetId="6" r:id="rId4"/>
+    <sheet name="gradientFill" sheetId="7" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="intersection">Sheet1!$B:$B Sheet1!$8:$8</definedName>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="182">
   <si>
     <t>normal</t>
   </si>
@@ -864,6 +865,72 @@
   <si>
     <t>tint</t>
   </si>
+  <si>
+    <t>Two-colour fill</t>
+  </si>
+  <si>
+    <t>Fill Horizontal Variant 2</t>
+  </si>
+  <si>
+    <t>Fill Horizontal Variant 3</t>
+  </si>
+  <si>
+    <t>Fill vertical variant 2</t>
+  </si>
+  <si>
+    <t>Fill vertical variant 3</t>
+  </si>
+  <si>
+    <t>Fill diagonal up variant 2</t>
+  </si>
+  <si>
+    <t>Fill diagonal up variant 3</t>
+  </si>
+  <si>
+    <t>Fill diagonal down variant 2</t>
+  </si>
+  <si>
+    <t>Fill diagonal down variant 3</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 2</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 3</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 4</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>stop1 positon</t>
+  </si>
+  <si>
+    <t>stop2 position</t>
+  </si>
+  <si>
+    <t>Fill Horizontal</t>
+  </si>
 </sst>
 </file>
 
@@ -1250,7 +1317,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1444,8 +1511,140 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+        <stop position="0">
+          <color theme="9"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="270">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="180">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="225">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="45">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="315">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="135">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" left="1" right="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" top="1" bottom="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" left="1" right="1" top="1" bottom="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1560,6 +1759,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1572,7 +1800,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1665,15 +1893,52 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1750,11 +2015,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="125910016"/>
-        <c:axId val="128404864"/>
+        <c:axId val="126473728"/>
+        <c:axId val="126475264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="125910016"/>
+        <c:axId val="126473728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +2028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128404864"/>
+        <c:crossAx val="126475264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +2036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128404864"/>
+        <c:axId val="126475264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,13 +2047,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125910016"/>
+        <c:crossAx val="126473728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1802,7 +2068,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1813,7 +2079,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308171" cy="6078963"/>
+    <xdr:ext cx="9225868" cy="6029876"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2146,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2501,7 +2767,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="79" t="s">
+      <c r="A42" s="85" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2509,7 +2775,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="79"/>
+      <c r="A43" s="85"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3144,7 +3410,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A133" s="80" t="s">
+      <c r="A133" s="79" t="s">
         <v>154</v>
       </c>
       <c r="B133" t="s">
@@ -3152,7 +3418,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A134" s="81" t="s">
+      <c r="A134" s="80" t="s">
         <v>155</v>
       </c>
       <c r="B134" t="s">
@@ -3160,7 +3426,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="82" t="s">
+      <c r="A135" s="81" t="s">
         <v>156</v>
       </c>
       <c r="B135" t="s">
@@ -3168,7 +3434,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A136" s="83" t="s">
+      <c r="A136" s="82" t="s">
         <v>157</v>
       </c>
       <c r="B136" t="s">
@@ -3176,7 +3442,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A137" s="84" t="s">
+      <c r="A137" s="83" t="s">
         <v>158</v>
       </c>
       <c r="B137" t="s">
@@ -3184,11 +3450,83 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="85" t="s">
+      <c r="A138" s="84" t="s">
         <v>159</v>
       </c>
       <c r="B138" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="86"/>
+      <c r="B139" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="87"/>
+      <c r="B140" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="88"/>
+      <c r="B141" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="89"/>
+      <c r="B142" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="90"/>
+      <c r="B143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="91"/>
+      <c r="B144" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="92"/>
+      <c r="B145" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="93"/>
+      <c r="B146" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="94"/>
+      <c r="B147" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="95"/>
+      <c r="B148" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="96"/>
+      <c r="B149" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="97"/>
+      <c r="B150" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -3294,4 +3632,453 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="110"/>
+      <c r="B3" s="99" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="99">
+        <v>0</v>
+      </c>
+      <c r="D3" s="99">
+        <v>1</v>
+      </c>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99">
+        <v>90</v>
+      </c>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="100"/>
+    </row>
+    <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="111"/>
+      <c r="B4" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="102">
+        <v>0</v>
+      </c>
+      <c r="D4" s="102">
+        <v>1</v>
+      </c>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102">
+        <v>270</v>
+      </c>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
+    </row>
+    <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="112"/>
+      <c r="B5" s="105" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="105">
+        <v>0</v>
+      </c>
+      <c r="D5" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105">
+        <v>90</v>
+      </c>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="106"/>
+    </row>
+    <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="107"/>
+      <c r="B7" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="99">
+        <v>0</v>
+      </c>
+      <c r="D7" s="99">
+        <v>1</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="100"/>
+    </row>
+    <row r="8" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="108"/>
+      <c r="B8" s="102" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="122">
+        <v>0</v>
+      </c>
+      <c r="D8" s="122">
+        <v>1</v>
+      </c>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102">
+        <v>180</v>
+      </c>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="103"/>
+    </row>
+    <row r="9" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="109"/>
+      <c r="B9" s="105" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="105">
+        <v>0</v>
+      </c>
+      <c r="D9" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+    </row>
+    <row r="10" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="122"/>
+    </row>
+    <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="98"/>
+      <c r="B11" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="99">
+        <v>0</v>
+      </c>
+      <c r="D11" s="99">
+        <v>1</v>
+      </c>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99">
+        <v>45</v>
+      </c>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="100"/>
+    </row>
+    <row r="12" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="101"/>
+      <c r="B12" s="102" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="122">
+        <v>0</v>
+      </c>
+      <c r="D12" s="122">
+        <v>1</v>
+      </c>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102">
+        <v>225</v>
+      </c>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="103"/>
+    </row>
+    <row r="13" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="104"/>
+      <c r="B13" s="105" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="105">
+        <v>0</v>
+      </c>
+      <c r="D13" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105">
+        <v>45</v>
+      </c>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="106"/>
+    </row>
+    <row r="14" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="113"/>
+      <c r="B15" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="99">
+        <v>0</v>
+      </c>
+      <c r="D15" s="99">
+        <v>1</v>
+      </c>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99">
+        <v>135</v>
+      </c>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="100"/>
+    </row>
+    <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="114"/>
+      <c r="B16" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="122">
+        <v>0</v>
+      </c>
+      <c r="D16" s="122">
+        <v>1</v>
+      </c>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102">
+        <v>315</v>
+      </c>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="103"/>
+    </row>
+    <row r="17" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="115"/>
+      <c r="B17" s="105" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="105">
+        <v>0</v>
+      </c>
+      <c r="D17" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105">
+        <v>135</v>
+      </c>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="106"/>
+    </row>
+    <row r="18" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="116"/>
+      <c r="B19" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="99">
+        <v>0</v>
+      </c>
+      <c r="D19" s="99">
+        <v>1</v>
+      </c>
+      <c r="E19" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="100"/>
+    </row>
+    <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="117"/>
+      <c r="B20" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="122">
+        <v>0</v>
+      </c>
+      <c r="D20" s="122">
+        <v>1</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102">
+        <v>1</v>
+      </c>
+      <c r="H20" s="102">
+        <v>1</v>
+      </c>
+      <c r="I20" s="102"/>
+      <c r="J20" s="103"/>
+    </row>
+    <row r="21" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="118"/>
+      <c r="B21" s="102" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="122">
+        <v>0</v>
+      </c>
+      <c r="D21" s="122">
+        <v>1</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102">
+        <v>1</v>
+      </c>
+      <c r="J21" s="103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="119"/>
+      <c r="B22" s="105" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="105">
+        <v>0</v>
+      </c>
+      <c r="D22" s="105">
+        <v>1</v>
+      </c>
+      <c r="E22" s="105" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105">
+        <v>1</v>
+      </c>
+      <c r="H22" s="105">
+        <v>1</v>
+      </c>
+      <c r="I22" s="105">
+        <v>1</v>
+      </c>
+      <c r="J22" s="106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="120"/>
+      <c r="B24" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="99">
+        <v>0</v>
+      </c>
+      <c r="D24" s="99">
+        <v>1</v>
+      </c>
+      <c r="E24" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="H24" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="100">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="121"/>
+      <c r="B25" s="105" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="105">
+        <v>0</v>
+      </c>
+      <c r="D25" s="105">
+        <v>1</v>
+      </c>
+      <c r="E25" s="105" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="106">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete tests of borders
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -1644,7 +1644,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1788,6 +1788,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDotDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1800,7 +1935,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1899,9 +2034,6 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
@@ -1939,6 +2071,24 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2015,11 +2165,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="126473728"/>
-        <c:axId val="126475264"/>
+        <c:axId val="128350848"/>
+        <c:axId val="128895232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126473728"/>
+        <c:axId val="128350848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126475264"/>
+        <c:crossAx val="128895232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2036,7 +2186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126475264"/>
+        <c:axId val="128895232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,14 +2197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126473728"/>
+        <c:crossAx val="128350848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2412,11 +2561,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B150"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2767,7 +2914,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="122" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2775,7 +2922,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="85"/>
+      <c r="A43" s="122"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3458,76 +3605,124 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="86"/>
+      <c r="A139" s="85"/>
       <c r="B139" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="87"/>
+      <c r="A140" s="86"/>
       <c r="B140" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="88"/>
+      <c r="A141" s="87"/>
       <c r="B141" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="89"/>
+      <c r="A142" s="88"/>
       <c r="B142" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="90"/>
+      <c r="A143" s="89"/>
       <c r="B143" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="91"/>
+      <c r="A144" s="90"/>
       <c r="B144" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="92"/>
+      <c r="A145" s="91"/>
       <c r="B145" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="93"/>
+      <c r="A146" s="92"/>
       <c r="B146" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="94"/>
+      <c r="A147" s="93"/>
       <c r="B147" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="95"/>
+      <c r="A148" s="94"/>
       <c r="B148" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="96"/>
+      <c r="A149" s="95"/>
       <c r="B149" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="97"/>
+      <c r="A150" s="96"/>
       <c r="B150" t="s">
         <v>171</v>
       </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="123"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="124"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="125"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="126"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="127"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="102"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="128"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="129"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="130"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="131"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="132"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="133"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="134"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="135"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="136"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3684,397 +3879,397 @@
     </row>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="110"/>
-      <c r="B3" s="99" t="s">
+      <c r="A3" s="109"/>
+      <c r="B3" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="99">
+      <c r="C3" s="98">
         <v>0</v>
       </c>
-      <c r="D3" s="99">
+      <c r="D3" s="98">
         <v>1</v>
       </c>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99">
+      <c r="E3" s="98"/>
+      <c r="F3" s="98">
         <v>90</v>
       </c>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="100"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="111"/>
-      <c r="B4" s="102" t="s">
+      <c r="A4" s="110"/>
+      <c r="B4" s="101" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="102">
+      <c r="C4" s="101">
         <v>0</v>
       </c>
-      <c r="D4" s="102">
+      <c r="D4" s="101">
         <v>1</v>
       </c>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102">
+      <c r="E4" s="101"/>
+      <c r="F4" s="101">
         <v>270</v>
       </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="112"/>
-      <c r="B5" s="105" t="s">
+      <c r="A5" s="111"/>
+      <c r="B5" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5" s="104">
         <v>0</v>
       </c>
-      <c r="D5" s="105">
+      <c r="D5" s="104">
         <v>0.5</v>
       </c>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105">
+      <c r="E5" s="104"/>
+      <c r="F5" s="104">
         <v>90</v>
       </c>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="106"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="105"/>
     </row>
     <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="107"/>
-      <c r="B7" s="99" t="s">
+      <c r="A7" s="106"/>
+      <c r="B7" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="98">
         <v>0</v>
       </c>
-      <c r="D7" s="99">
+      <c r="D7" s="98">
         <v>1</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="100"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="99"/>
     </row>
     <row r="8" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="108"/>
-      <c r="B8" s="102" t="s">
+      <c r="A8" s="107"/>
+      <c r="B8" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="122">
+      <c r="C8" s="121">
         <v>0</v>
       </c>
-      <c r="D8" s="122">
+      <c r="D8" s="121">
         <v>1</v>
       </c>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102">
+      <c r="E8" s="101"/>
+      <c r="F8" s="101">
         <v>180</v>
       </c>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="103"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="102"/>
     </row>
     <row r="9" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="109"/>
-      <c r="B9" s="105" t="s">
+      <c r="A9" s="108"/>
+      <c r="B9" s="104" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="105">
+      <c r="C9" s="104">
         <v>0</v>
       </c>
-      <c r="D9" s="105">
+      <c r="D9" s="104">
         <v>0.5</v>
       </c>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="106"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="122"/>
+      <c r="C10" s="121"/>
     </row>
     <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="98"/>
-      <c r="B11" s="99" t="s">
+      <c r="A11" s="97"/>
+      <c r="B11" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="99">
+      <c r="C11" s="98">
         <v>0</v>
       </c>
-      <c r="D11" s="99">
+      <c r="D11" s="98">
         <v>1</v>
       </c>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99">
+      <c r="E11" s="98"/>
+      <c r="F11" s="98">
         <v>45</v>
       </c>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="100"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="101"/>
-      <c r="B12" s="102" t="s">
+      <c r="A12" s="100"/>
+      <c r="B12" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="122">
+      <c r="C12" s="121">
         <v>0</v>
       </c>
-      <c r="D12" s="122">
+      <c r="D12" s="121">
         <v>1</v>
       </c>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102">
+      <c r="E12" s="101"/>
+      <c r="F12" s="101">
         <v>225</v>
       </c>
-      <c r="G12" s="102"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="103"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="102"/>
     </row>
     <row r="13" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="105" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="104" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="104">
         <v>0</v>
       </c>
-      <c r="D13" s="105">
+      <c r="D13" s="104">
         <v>0.5</v>
       </c>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105">
+      <c r="E13" s="104"/>
+      <c r="F13" s="104">
         <v>45</v>
       </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="106"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="105"/>
     </row>
     <row r="14" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="113"/>
-      <c r="B15" s="99" t="s">
+      <c r="A15" s="112"/>
+      <c r="B15" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="99">
+      <c r="C15" s="98">
         <v>0</v>
       </c>
-      <c r="D15" s="99">
+      <c r="D15" s="98">
         <v>1</v>
       </c>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99">
+      <c r="E15" s="98"/>
+      <c r="F15" s="98">
         <v>135</v>
       </c>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="100"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="99"/>
     </row>
     <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="114"/>
-      <c r="B16" s="102" t="s">
+      <c r="A16" s="113"/>
+      <c r="B16" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="122">
+      <c r="C16" s="121">
         <v>0</v>
       </c>
-      <c r="D16" s="122">
+      <c r="D16" s="121">
         <v>1</v>
       </c>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102">
+      <c r="E16" s="101"/>
+      <c r="F16" s="101">
         <v>315</v>
       </c>
-      <c r="G16" s="102"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="103"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="102"/>
     </row>
     <row r="17" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="115"/>
-      <c r="B17" s="105" t="s">
+      <c r="A17" s="114"/>
+      <c r="B17" s="104" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="105">
+      <c r="C17" s="104">
         <v>0</v>
       </c>
-      <c r="D17" s="105">
+      <c r="D17" s="104">
         <v>0.5</v>
       </c>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105">
+      <c r="E17" s="104"/>
+      <c r="F17" s="104">
         <v>135</v>
       </c>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="106"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="105"/>
     </row>
     <row r="18" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="116"/>
-      <c r="B19" s="99" t="s">
+      <c r="A19" s="115"/>
+      <c r="B19" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="99">
+      <c r="C19" s="98">
         <v>0</v>
       </c>
-      <c r="D19" s="99">
+      <c r="D19" s="98">
         <v>1</v>
       </c>
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="98" t="s">
         <v>172</v>
       </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="100"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="99"/>
     </row>
     <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="117"/>
-      <c r="B20" s="102" t="s">
+      <c r="A20" s="116"/>
+      <c r="B20" s="101" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="122">
+      <c r="C20" s="121">
         <v>0</v>
       </c>
-      <c r="D20" s="122">
+      <c r="D20" s="121">
         <v>1</v>
       </c>
-      <c r="E20" s="102" t="s">
+      <c r="E20" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102">
+      <c r="F20" s="101"/>
+      <c r="G20" s="101">
         <v>1</v>
       </c>
-      <c r="H20" s="102">
+      <c r="H20" s="101">
         <v>1</v>
       </c>
-      <c r="I20" s="102"/>
-      <c r="J20" s="103"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="102"/>
     </row>
     <row r="21" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="118"/>
-      <c r="B21" s="102" t="s">
+      <c r="A21" s="117"/>
+      <c r="B21" s="101" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="122">
+      <c r="C21" s="121">
         <v>0</v>
       </c>
-      <c r="D21" s="122">
+      <c r="D21" s="121">
         <v>1</v>
       </c>
-      <c r="E21" s="102" t="s">
+      <c r="E21" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="102">
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101">
         <v>1</v>
       </c>
-      <c r="J21" s="103">
+      <c r="J21" s="102">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="119"/>
-      <c r="B22" s="105" t="s">
+      <c r="A22" s="118"/>
+      <c r="B22" s="104" t="s">
         <v>171</v>
       </c>
-      <c r="C22" s="105">
+      <c r="C22" s="104">
         <v>0</v>
       </c>
-      <c r="D22" s="105">
+      <c r="D22" s="104">
         <v>1</v>
       </c>
-      <c r="E22" s="105" t="s">
+      <c r="E22" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105">
+      <c r="F22" s="104"/>
+      <c r="G22" s="104">
         <v>1</v>
       </c>
-      <c r="H22" s="105">
+      <c r="H22" s="104">
         <v>1</v>
       </c>
-      <c r="I22" s="105">
+      <c r="I22" s="104">
         <v>1</v>
       </c>
-      <c r="J22" s="106">
+      <c r="J22" s="105">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="120"/>
-      <c r="B24" s="99" t="s">
+      <c r="A24" s="119"/>
+      <c r="B24" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="99">
+      <c r="C24" s="98">
         <v>0</v>
       </c>
-      <c r="D24" s="99">
+      <c r="D24" s="98">
         <v>1</v>
       </c>
-      <c r="E24" s="99" t="s">
+      <c r="E24" s="98" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99">
+      <c r="F24" s="98"/>
+      <c r="G24" s="98">
         <v>0.5</v>
       </c>
-      <c r="H24" s="99">
+      <c r="H24" s="98">
         <v>0.5</v>
       </c>
-      <c r="I24" s="99">
+      <c r="I24" s="98">
         <v>0.5</v>
       </c>
-      <c r="J24" s="100">
+      <c r="J24" s="99">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="121"/>
-      <c r="B25" s="105" t="s">
+      <c r="A25" s="120"/>
+      <c r="B25" s="104" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="105">
+      <c r="C25" s="104">
         <v>0</v>
       </c>
-      <c r="D25" s="105">
+      <c r="D25" s="104">
         <v>1</v>
       </c>
-      <c r="E25" s="105" t="s">
+      <c r="E25" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105">
+      <c r="F25" s="104"/>
+      <c r="G25" s="104">
         <v>0.5</v>
       </c>
-      <c r="H25" s="105">
+      <c r="H25" s="104">
         <v>0.5</v>
       </c>
-      <c r="I25" s="105">
+      <c r="I25" s="104">
         <v>0.5</v>
       </c>
-      <c r="J25" s="106">
+      <c r="J25" s="105">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Annotate new border examples in xlsx file
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="196">
   <si>
     <t>normal</t>
   </si>
@@ -930,6 +930,48 @@
   </si>
   <si>
     <t>Fill Horizontal</t>
+  </si>
+  <si>
+    <t>hair</t>
+  </si>
+  <si>
+    <t>dotted</t>
+  </si>
+  <si>
+    <t>dashDotDot</t>
+  </si>
+  <si>
+    <t>dashed</t>
+  </si>
+  <si>
+    <t>mediumDashDotDot</t>
+  </si>
+  <si>
+    <t>slantDashDot</t>
+  </si>
+  <si>
+    <t>mediumDashDot</t>
+  </si>
+  <si>
+    <t>mediumDashed</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>thick</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>diagonalUp</t>
+  </si>
+  <si>
+    <t>diagonalDown</t>
+  </si>
+  <si>
+    <t>both diagonals (will always be the same style)</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1977,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2071,9 +2113,6 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -2089,6 +2128,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2165,11 +2208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128350848"/>
-        <c:axId val="128895232"/>
+        <c:axId val="132410368"/>
+        <c:axId val="133742976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128350848"/>
+        <c:axId val="132410368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,7 +2221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128895232"/>
+        <c:crossAx val="133742976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2186,7 +2229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128895232"/>
+        <c:axId val="133742976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,13 +2240,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128350848"/>
+        <c:crossAx val="132410368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2217,7 +2261,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="96" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2228,7 +2272,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9225868" cy="6029876"/>
+    <xdr:ext cx="9227344" cy="6022578"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2561,7 +2605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B166"/>
+  <dimension ref="A1:B167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2914,7 +2958,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="137" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2922,7 +2966,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="122"/>
+      <c r="A43" s="137"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3677,58 +3721,141 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="123"/>
+      <c r="A151" s="122" t="s">
+        <v>182</v>
+      </c>
+      <c r="B151" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="124"/>
+      <c r="A152" s="123" t="s">
+        <v>183</v>
+      </c>
+      <c r="B152" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="125"/>
+      <c r="A153" s="124" t="s">
+        <v>184</v>
+      </c>
+      <c r="B153" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="126"/>
+      <c r="A154" s="125" t="s">
+        <v>60</v>
+      </c>
+      <c r="B154" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="127"/>
+      <c r="A155" s="126" t="s">
+        <v>185</v>
+      </c>
+      <c r="B155" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="102"/>
+      <c r="A156" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="128"/>
+      <c r="A157" s="127" t="s">
+        <v>186</v>
+      </c>
+      <c r="B157" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="129"/>
+      <c r="A158" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B158" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="130"/>
+      <c r="A159" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="B159" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="131"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="132"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="133"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="134"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="135"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="136"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="137"/>
+      <c r="A160" s="130" t="s">
+        <v>189</v>
+      </c>
+      <c r="B160" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="131" t="s">
+        <v>190</v>
+      </c>
+      <c r="B161" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="132" t="s">
+        <v>191</v>
+      </c>
+      <c r="B162" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="133" t="s">
+        <v>192</v>
+      </c>
+      <c r="B163" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="134" t="s">
+        <v>193</v>
+      </c>
+      <c r="B164" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="135" t="s">
+        <v>194</v>
+      </c>
+      <c r="B165" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="136" t="s">
+        <v>195</v>
+      </c>
+      <c r="B166" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A42:A43"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="15">
+  <dataValidations count="15">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error title" error="error body" promptTitle="message title" prompt="message body" sqref="A106">
       <formula1>0</formula1>
       <formula2>9</formula2>

</xml_diff>

<commit_message>
Make format alignment defaults consistent
E.g. return FALSE rather than NA
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>normal</t>
   </si>
@@ -972,6 +972,69 @@
   </si>
   <si>
     <t>both diagonals (will always be the same style)</t>
+  </si>
+  <si>
+    <t>vertical align top</t>
+  </si>
+  <si>
+    <t>vertical align bottom</t>
+  </si>
+  <si>
+    <t>horizontal align left</t>
+  </si>
+  <si>
+    <t>horizontal align right</t>
+  </si>
+  <si>
+    <t>horizontal align center</t>
+  </si>
+  <si>
+    <t>indent</t>
+  </si>
+  <si>
+    <t>vertical align center</t>
+  </si>
+  <si>
+    <t>vertical align justify</t>
+  </si>
+  <si>
+    <t>vertical align distributed</t>
+  </si>
+  <si>
+    <t>horizontal align general</t>
+  </si>
+  <si>
+    <t>horizontal align fill</t>
+  </si>
+  <si>
+    <t>horizontal align justify</t>
+  </si>
+  <si>
+    <t>horizontal align center across selection</t>
+  </si>
+  <si>
+    <t>horizontal align distributed</t>
+  </si>
+  <si>
+    <t>wrap text</t>
+  </si>
+  <si>
+    <t>shrink to fit</t>
+  </si>
+  <si>
+    <t>merge cells</t>
+  </si>
+  <si>
+    <t>reading order context</t>
+  </si>
+  <si>
+    <t>reading order left to right</t>
+  </si>
+  <si>
+    <t>reading order right to left</t>
+  </si>
+  <si>
+    <t>text rotation</t>
   </si>
 </sst>
 </file>
@@ -1977,7 +2040,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2128,6 +2191,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="105"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
@@ -2208,11 +2319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132410368"/>
-        <c:axId val="133742976"/>
+        <c:axId val="129314176"/>
+        <c:axId val="131861888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132410368"/>
+        <c:axId val="129314176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133742976"/>
+        <c:crossAx val="131861888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2229,7 +2340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133742976"/>
+        <c:axId val="131861888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,14 +2351,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132410368"/>
+        <c:crossAx val="129314176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2605,9 +2715,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B167"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2958,7 +3070,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="137" t="s">
+      <c r="A42" s="153" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2966,7 +3078,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="137"/>
+      <c r="A43" s="153"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3800,7 +3912,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="131" t="s">
         <v>190</v>
       </c>
@@ -3808,7 +3920,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="132" t="s">
         <v>191</v>
       </c>
@@ -3816,7 +3928,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="133" t="s">
         <v>192</v>
       </c>
@@ -3824,7 +3936,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="134" t="s">
         <v>193</v>
       </c>
@@ -3832,7 +3944,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="135" t="s">
         <v>194</v>
       </c>
@@ -3840,7 +3952,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="136" t="s">
         <v>195</v>
       </c>
@@ -3848,14 +3960,182 @@
         <v>195</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="138"/>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>205</v>
+      </c>
+      <c r="B167" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="141" t="s">
+        <v>198</v>
+      </c>
+      <c r="B168" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="140" t="s">
+        <v>200</v>
+      </c>
+      <c r="B169" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="139" t="s">
+        <v>199</v>
+      </c>
+      <c r="B170" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="145" t="s">
+        <v>206</v>
+      </c>
+      <c r="B171" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="146" t="s">
+        <v>207</v>
+      </c>
+      <c r="B172" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="B173" s="147"/>
+      <c r="D173" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="E173" s="147"/>
+      <c r="F173" s="147"/>
+      <c r="G173" s="147"/>
+    </row>
+    <row r="174" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A174" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="B174" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="137" t="s">
+        <v>196</v>
+      </c>
+      <c r="B175" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="138" t="s">
+        <v>202</v>
+      </c>
+      <c r="B176" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>197</v>
+      </c>
+      <c r="B177" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="143" t="s">
+        <v>203</v>
+      </c>
+      <c r="B178" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A179" s="144" t="s">
+        <v>204</v>
+      </c>
+      <c r="B179" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="B180" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B181" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="149" t="s">
+        <v>211</v>
+      </c>
+      <c r="B182" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="154" t="s">
+        <v>212</v>
+      </c>
+      <c r="B183" s="154"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>213</v>
+      </c>
+      <c r="B184" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="150" t="s">
+        <v>214</v>
+      </c>
+      <c r="B185" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="151" t="s">
+        <v>215</v>
+      </c>
+      <c r="B186" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="30.75" x14ac:dyDescent="0.2">
+      <c r="A187" s="152" t="s">
+        <v>216</v>
+      </c>
+      <c r="B187" t="s">
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A183:B183"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations disablePrompts="1" count="15">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error title" error="error body" promptTitle="message title" prompt="message body" sqref="A106">
       <formula1>0</formula1>
       <formula2>9</formula2>

</xml_diff>

<commit_message>
Add indexed colours to examples.xlsx
It shows that they aren't saved as indexed colours, only RGB values.
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="236">
   <si>
     <t>normal</t>
   </si>
@@ -1042,6 +1042,57 @@
   <si>
     <t>a cell that is 'hidden'</t>
   </si>
+  <si>
+    <t>background1</t>
+  </si>
+  <si>
+    <t>background1 theme colour</t>
+  </si>
+  <si>
+    <t>text1 lighter 50%</t>
+  </si>
+  <si>
+    <t>text1 lighter 35%</t>
+  </si>
+  <si>
+    <t>text1 lighter 25%</t>
+  </si>
+  <si>
+    <t>text1 lighter 15%</t>
+  </si>
+  <si>
+    <t>text1 lighter 5%</t>
+  </si>
+  <si>
+    <t>standared red</t>
+  </si>
+  <si>
+    <t>standard dark red</t>
+  </si>
+  <si>
+    <t>standard orange</t>
+  </si>
+  <si>
+    <t>standared yellow</t>
+  </si>
+  <si>
+    <t>standard light green</t>
+  </si>
+  <si>
+    <t>standard green</t>
+  </si>
+  <si>
+    <t>standard light blue</t>
+  </si>
+  <si>
+    <t>standard blue</t>
+  </si>
+  <si>
+    <t>standard dark blue</t>
+  </si>
+  <si>
+    <t>standard purple</t>
+  </si>
 </sst>
 </file>
 
@@ -1054,11 +1105,18 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="69" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1424,6 +1482,102 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2037,47 +2191,47 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -2097,38 +2251,38 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2137,14 +2291,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
@@ -2249,10 +2403,27 @@
       <alignment readingOrder="2"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2329,11 +2500,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128652032"/>
-        <c:axId val="128653568"/>
+        <c:axId val="130815488"/>
+        <c:axId val="130817024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128652032"/>
+        <c:axId val="130815488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2342,7 +2513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128653568"/>
+        <c:crossAx val="130817024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2350,7 +2521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128653568"/>
+        <c:axId val="130817024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2361,7 +2532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128652032"/>
+        <c:crossAx val="130815488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2725,10 +2896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G188"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A121" activeCellId="1" sqref="A115 A121:A122"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195:B204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4146,6 +4317,134 @@
       </c>
       <c r="B188" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A189" s="156" t="s">
+        <v>219</v>
+      </c>
+      <c r="B189" s="157" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="B190" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="B191" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="160" t="s">
+        <v>223</v>
+      </c>
+      <c r="B192" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="161" t="s">
+        <v>224</v>
+      </c>
+      <c r="B193" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="B194" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="166" t="s">
+        <v>227</v>
+      </c>
+      <c r="B195" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="165" t="s">
+        <v>226</v>
+      </c>
+      <c r="B196" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="164" t="s">
+        <v>228</v>
+      </c>
+      <c r="B197" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="163" t="s">
+        <v>229</v>
+      </c>
+      <c r="B198" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="168" t="s">
+        <v>230</v>
+      </c>
+      <c r="B199" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="167" t="s">
+        <v>231</v>
+      </c>
+      <c r="B200" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="169" t="s">
+        <v>232</v>
+      </c>
+      <c r="B201" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="170" t="s">
+        <v>233</v>
+      </c>
+      <c r="B202" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="171" t="s">
+        <v>234</v>
+      </c>
+      <c r="B203" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="172" t="s">
+        <v>235</v>
+      </c>
+      <c r="B204" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use names for theme colours rather than numbers
E.g. `"accent6"` instead of `4`
</commit_message>
<xml_diff>
--- a/tests/testthat/examples.xlsx
+++ b/tests/testthat/examples.xlsx
@@ -1105,7 +1105,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="69" x14ac:knownFonts="1">
+  <fonts count="70" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -1578,6 +1578,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2252,7 +2258,6 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2403,10 +2408,6 @@
       <alignment readingOrder="2"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2424,6 +2425,11 @@
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2500,11 +2506,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="130815488"/>
-        <c:axId val="130817024"/>
+        <c:axId val="87340544"/>
+        <c:axId val="87342080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130815488"/>
+        <c:axId val="87340544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2513,7 +2519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130817024"/>
+        <c:crossAx val="87342080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2521,7 +2527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130817024"/>
+        <c:axId val="87342080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2532,7 +2538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130815488"/>
+        <c:crossAx val="87340544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2898,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195:B204"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3032,7 +3038,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="74">
+      <c r="A16" s="73">
         <f>DATE(2017,1,18)</f>
         <v>42753</v>
       </c>
@@ -3126,7 +3132,7 @@
       <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="70" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3139,7 +3145,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="64" t="s">
         <v>0</v>
       </c>
       <c r="B28" t="s">
@@ -3147,7 +3153,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
@@ -3155,7 +3161,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="63" t="s">
         <v>0</v>
       </c>
       <c r="B30" t="s">
@@ -3235,7 +3241,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
@@ -3243,7 +3249,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="54" t="s">
         <v>7</v>
       </c>
       <c r="B41" t="s">
@@ -3251,7 +3257,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="154" t="s">
+      <c r="A42" s="170" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -3259,7 +3265,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="154"/>
+      <c r="A43" s="170"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3270,7 +3276,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="72" t="s">
+      <c r="A45" s="71" t="s">
         <v>110</v>
       </c>
       <c r="B45" t="s">
@@ -3278,7 +3284,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="73" t="s">
+      <c r="A46" s="72" t="s">
         <v>112</v>
       </c>
       <c r="B46" t="s">
@@ -3326,7 +3332,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="55" t="s">
         <v>31</v>
       </c>
       <c r="B52" t="s">
@@ -3334,130 +3340,130 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="67" t="s">
+      <c r="B53" s="66" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="68" t="s">
+      <c r="B54" s="67" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="69" t="s">
+      <c r="B55" s="68" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="57" t="s">
+      <c r="A56" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B56" s="66" t="s">
+      <c r="B56" s="65" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="42" t="s">
+      <c r="A57" s="172" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="70" t="s">
+      <c r="B57" s="69" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="70" t="s">
+      <c r="B58" s="69" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="70" t="s">
+      <c r="B59" s="69" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="70" t="s">
+      <c r="B60" s="69" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="46" t="s">
+      <c r="A61" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B61" s="69" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="70" t="s">
+      <c r="B62" s="69" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="48" t="s">
+      <c r="A63" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B63" s="70" t="s">
+      <c r="B63" s="69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B64" s="70" t="s">
+      <c r="B64" s="69" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="50" t="s">
+      <c r="A65" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B65" s="69" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="51" t="s">
+      <c r="A66" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B66" s="70" t="s">
+      <c r="B66" s="69" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="52" t="s">
+      <c r="A67" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B67" s="70" t="s">
+      <c r="B67" s="69" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="53" t="s">
+      <c r="A68" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B68" s="70" t="s">
+      <c r="B68" s="69" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3576,37 +3582,37 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="58"/>
+      <c r="A88" s="57"/>
       <c r="B88" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="59"/>
+      <c r="A89" s="58"/>
       <c r="B89" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="60"/>
+      <c r="A90" s="59"/>
       <c r="B90" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="61"/>
+      <c r="A91" s="60"/>
       <c r="B91" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="62"/>
+      <c r="A92" s="61"/>
       <c r="B92" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="63"/>
+      <c r="A93" s="62"/>
       <c r="B93" t="s">
         <v>105</v>
       </c>
@@ -3620,7 +3626,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="75">
+      <c r="A95" s="74">
         <v>-1</v>
       </c>
       <c r="B95" t="s">
@@ -3732,7 +3738,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="74">
+      <c r="A110" s="73">
         <v>42736</v>
       </c>
       <c r="B110" t="s">
@@ -3740,7 +3746,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="76">
+      <c r="A111" s="75">
         <v>0.35416666666666669</v>
       </c>
       <c r="B111" t="s">
@@ -3886,7 +3892,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="77" t="s">
+      <c r="A132" s="76" t="s">
         <v>153</v>
       </c>
       <c r="B132" t="s">
@@ -3894,7 +3900,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A133" s="79" t="s">
+      <c r="A133" s="78" t="s">
         <v>154</v>
       </c>
       <c r="B133" t="s">
@@ -3902,7 +3908,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A134" s="80" t="s">
+      <c r="A134" s="79" t="s">
         <v>155</v>
       </c>
       <c r="B134" t="s">
@@ -3910,7 +3916,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="81" t="s">
+      <c r="A135" s="80" t="s">
         <v>156</v>
       </c>
       <c r="B135" t="s">
@@ -3918,7 +3924,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A136" s="82" t="s">
+      <c r="A136" s="81" t="s">
         <v>157</v>
       </c>
       <c r="B136" t="s">
@@ -3926,7 +3932,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A137" s="83" t="s">
+      <c r="A137" s="82" t="s">
         <v>158</v>
       </c>
       <c r="B137" t="s">
@@ -3934,7 +3940,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="84" t="s">
+      <c r="A138" s="83" t="s">
         <v>159</v>
       </c>
       <c r="B138" t="s">
@@ -3942,79 +3948,79 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="85"/>
+      <c r="A139" s="84"/>
       <c r="B139" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="86"/>
+      <c r="A140" s="85"/>
       <c r="B140" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="87"/>
+      <c r="A141" s="86"/>
       <c r="B141" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="88"/>
+      <c r="A142" s="87"/>
       <c r="B142" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="89"/>
+      <c r="A143" s="88"/>
       <c r="B143" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="90"/>
+      <c r="A144" s="89"/>
       <c r="B144" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="91"/>
+      <c r="A145" s="90"/>
       <c r="B145" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="92"/>
+      <c r="A146" s="91"/>
       <c r="B146" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="93"/>
+      <c r="A147" s="92"/>
       <c r="B147" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="94"/>
+      <c r="A148" s="93"/>
       <c r="B148" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="95"/>
+      <c r="A149" s="94"/>
       <c r="B149" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="96"/>
+      <c r="A150" s="95"/>
       <c r="B150" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="122" t="s">
+      <c r="A151" s="121" t="s">
         <v>182</v>
       </c>
       <c r="B151" t="s">
@@ -4022,7 +4028,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="123" t="s">
+      <c r="A152" s="122" t="s">
         <v>183</v>
       </c>
       <c r="B152" t="s">
@@ -4030,7 +4036,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="124" t="s">
+      <c r="A153" s="123" t="s">
         <v>184</v>
       </c>
       <c r="B153" t="s">
@@ -4038,7 +4044,7 @@
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="125" t="s">
+      <c r="A154" s="124" t="s">
         <v>60</v>
       </c>
       <c r="B154" t="s">
@@ -4046,7 +4052,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="126" t="s">
+      <c r="A155" s="125" t="s">
         <v>185</v>
       </c>
       <c r="B155" t="s">
@@ -4054,7 +4060,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="102" t="s">
+      <c r="A156" s="101" t="s">
         <v>31</v>
       </c>
       <c r="B156" t="s">
@@ -4062,7 +4068,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="127" t="s">
+      <c r="A157" s="126" t="s">
         <v>186</v>
       </c>
       <c r="B157" t="s">
@@ -4070,7 +4076,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="128" t="s">
+      <c r="A158" s="127" t="s">
         <v>187</v>
       </c>
       <c r="B158" t="s">
@@ -4078,7 +4084,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="129" t="s">
+      <c r="A159" s="128" t="s">
         <v>188</v>
       </c>
       <c r="B159" t="s">
@@ -4086,7 +4092,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="130" t="s">
+      <c r="A160" s="129" t="s">
         <v>189</v>
       </c>
       <c r="B160" t="s">
@@ -4094,7 +4100,7 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A161" s="131" t="s">
+      <c r="A161" s="130" t="s">
         <v>190</v>
       </c>
       <c r="B161" t="s">
@@ -4102,7 +4108,7 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A162" s="132" t="s">
+      <c r="A162" s="131" t="s">
         <v>191</v>
       </c>
       <c r="B162" t="s">
@@ -4110,7 +4116,7 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" s="133" t="s">
+      <c r="A163" s="132" t="s">
         <v>192</v>
       </c>
       <c r="B163" t="s">
@@ -4118,7 +4124,7 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" s="134" t="s">
+      <c r="A164" s="133" t="s">
         <v>193</v>
       </c>
       <c r="B164" t="s">
@@ -4126,7 +4132,7 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" s="135" t="s">
+      <c r="A165" s="134" t="s">
         <v>194</v>
       </c>
       <c r="B165" t="s">
@@ -4134,7 +4140,7 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A166" s="136" t="s">
+      <c r="A166" s="135" t="s">
         <v>195</v>
       </c>
       <c r="B166" t="s">
@@ -4150,7 +4156,7 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A168" s="141" t="s">
+      <c r="A168" s="140" t="s">
         <v>198</v>
       </c>
       <c r="B168" t="s">
@@ -4158,7 +4164,7 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A169" s="140" t="s">
+      <c r="A169" s="139" t="s">
         <v>200</v>
       </c>
       <c r="B169" t="s">
@@ -4166,7 +4172,7 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A170" s="139" t="s">
+      <c r="A170" s="138" t="s">
         <v>199</v>
       </c>
       <c r="B170" t="s">
@@ -4174,7 +4180,7 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A171" s="145" t="s">
+      <c r="A171" s="144" t="s">
         <v>206</v>
       </c>
       <c r="B171" t="s">
@@ -4182,7 +4188,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A172" s="146" t="s">
+      <c r="A172" s="145" t="s">
         <v>207</v>
       </c>
       <c r="B172" t="s">
@@ -4190,19 +4196,19 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="147" t="s">
+      <c r="A173" s="146" t="s">
         <v>208</v>
       </c>
-      <c r="B173" s="147"/>
-      <c r="D173" s="147" t="s">
+      <c r="B173" s="146"/>
+      <c r="D173" s="146" t="s">
         <v>208</v>
       </c>
-      <c r="E173" s="147"/>
-      <c r="F173" s="147"/>
-      <c r="G173" s="147"/>
+      <c r="E173" s="146"/>
+      <c r="F173" s="146"/>
+      <c r="G173" s="146"/>
     </row>
     <row r="174" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A174" s="148" t="s">
+      <c r="A174" s="147" t="s">
         <v>209</v>
       </c>
       <c r="B174" t="s">
@@ -4210,7 +4216,7 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A175" s="137" t="s">
+      <c r="A175" s="136" t="s">
         <v>196</v>
       </c>
       <c r="B175" t="s">
@@ -4218,7 +4224,7 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A176" s="138" t="s">
+      <c r="A176" s="137" t="s">
         <v>202</v>
       </c>
       <c r="B176" t="s">
@@ -4234,7 +4240,7 @@
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="143" t="s">
+      <c r="A178" s="142" t="s">
         <v>203</v>
       </c>
       <c r="B178" t="s">
@@ -4242,7 +4248,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A179" s="144" t="s">
+      <c r="A179" s="143" t="s">
         <v>204</v>
       </c>
       <c r="B179" t="s">
@@ -4250,7 +4256,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="142" t="s">
+      <c r="A180" s="141" t="s">
         <v>201</v>
       </c>
       <c r="B180" t="s">
@@ -4266,7 +4272,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="149" t="s">
+      <c r="A182" s="148" t="s">
         <v>211</v>
       </c>
       <c r="B182" t="s">
@@ -4274,10 +4280,10 @@
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="155" t="s">
+      <c r="A183" s="171" t="s">
         <v>212</v>
       </c>
-      <c r="B183" s="155"/>
+      <c r="B183" s="171"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -4288,7 +4294,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="150" t="s">
+      <c r="A185" s="149" t="s">
         <v>214</v>
       </c>
       <c r="B185" t="s">
@@ -4296,7 +4302,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="151" t="s">
+      <c r="A186" s="150" t="s">
         <v>215</v>
       </c>
       <c r="B186" t="s">
@@ -4304,7 +4310,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" ht="30.75" x14ac:dyDescent="0.2">
-      <c r="A187" s="152" t="s">
+      <c r="A187" s="151" t="s">
         <v>216</v>
       </c>
       <c r="B187" t="s">
@@ -4312,7 +4318,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="153" t="s">
+      <c r="A188" s="152" t="s">
         <v>217</v>
       </c>
       <c r="B188" t="s">
@@ -4320,15 +4326,15 @@
       </c>
     </row>
     <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A189" s="156" t="s">
+      <c r="A189" s="153" t="s">
         <v>219</v>
       </c>
-      <c r="B189" s="157" t="s">
+      <c r="B189" s="154" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="158" t="s">
+      <c r="A190" s="155" t="s">
         <v>221</v>
       </c>
       <c r="B190" t="s">
@@ -4336,7 +4342,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="159" t="s">
+      <c r="A191" s="156" t="s">
         <v>222</v>
       </c>
       <c r="B191" t="s">
@@ -4344,7 +4350,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="160" t="s">
+      <c r="A192" s="157" t="s">
         <v>223</v>
       </c>
       <c r="B192" t="s">
@@ -4352,7 +4358,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="161" t="s">
+      <c r="A193" s="158" t="s">
         <v>224</v>
       </c>
       <c r="B193" t="s">
@@ -4360,7 +4366,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="162" t="s">
+      <c r="A194" s="159" t="s">
         <v>225</v>
       </c>
       <c r="B194" t="s">
@@ -4368,7 +4374,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="166" t="s">
+      <c r="A195" s="163" t="s">
         <v>227</v>
       </c>
       <c r="B195" t="s">
@@ -4376,7 +4382,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="165" t="s">
+      <c r="A196" s="162" t="s">
         <v>226</v>
       </c>
       <c r="B196" t="s">
@@ -4384,7 +4390,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="164" t="s">
+      <c r="A197" s="161" t="s">
         <v>228</v>
       </c>
       <c r="B197" t="s">
@@ -4392,7 +4398,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="163" t="s">
+      <c r="A198" s="160" t="s">
         <v>229</v>
       </c>
       <c r="B198" t="s">
@@ -4400,7 +4406,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="168" t="s">
+      <c r="A199" s="165" t="s">
         <v>230</v>
       </c>
       <c r="B199" t="s">
@@ -4408,7 +4414,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="167" t="s">
+      <c r="A200" s="164" t="s">
         <v>231</v>
       </c>
       <c r="B200" t="s">
@@ -4416,7 +4422,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="169" t="s">
+      <c r="A201" s="166" t="s">
         <v>232</v>
       </c>
       <c r="B201" t="s">
@@ -4424,7 +4430,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="170" t="s">
+      <c r="A202" s="167" t="s">
         <v>233</v>
       </c>
       <c r="B202" t="s">
@@ -4432,7 +4438,7 @@
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="171" t="s">
+      <c r="A203" s="168" t="s">
         <v>234</v>
       </c>
       <c r="B203" t="s">
@@ -4440,7 +4446,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="172" t="s">
+      <c r="A204" s="169" t="s">
         <v>235</v>
       </c>
       <c r="B204" t="s">
@@ -4603,397 +4609,397 @@
     </row>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="109"/>
-      <c r="B3" s="98" t="s">
+      <c r="A3" s="108"/>
+      <c r="B3" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="98">
+      <c r="C3" s="97">
         <v>0</v>
       </c>
-      <c r="D3" s="98">
+      <c r="D3" s="97">
         <v>1</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97">
         <v>90</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="98"/>
     </row>
     <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="110"/>
-      <c r="B4" s="101" t="s">
+      <c r="A4" s="109"/>
+      <c r="B4" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="101">
+      <c r="C4" s="100">
         <v>0</v>
       </c>
-      <c r="D4" s="101">
+      <c r="D4" s="100">
         <v>1</v>
       </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101">
+      <c r="E4" s="100"/>
+      <c r="F4" s="100">
         <v>270</v>
       </c>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="101"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="111"/>
-      <c r="B5" s="104" t="s">
+      <c r="A5" s="110"/>
+      <c r="B5" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="104">
+      <c r="C5" s="103">
         <v>0</v>
       </c>
-      <c r="D5" s="104">
+      <c r="D5" s="103">
         <v>0.5</v>
       </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104">
+      <c r="E5" s="103"/>
+      <c r="F5" s="103">
         <v>90</v>
       </c>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="105"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="104"/>
     </row>
     <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106"/>
-      <c r="B7" s="98" t="s">
+      <c r="A7" s="105"/>
+      <c r="B7" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="98">
+      <c r="C7" s="97">
         <v>0</v>
       </c>
-      <c r="D7" s="98">
+      <c r="D7" s="97">
         <v>1</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="99"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
     </row>
     <row r="8" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="107"/>
-      <c r="B8" s="101" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="100" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="121">
+      <c r="C8" s="120">
         <v>0</v>
       </c>
-      <c r="D8" s="121">
+      <c r="D8" s="120">
         <v>1</v>
       </c>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101">
+      <c r="E8" s="100"/>
+      <c r="F8" s="100">
         <v>180</v>
       </c>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="102"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="101"/>
     </row>
     <row r="9" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="108"/>
-      <c r="B9" s="104" t="s">
+      <c r="A9" s="107"/>
+      <c r="B9" s="103" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="104">
+      <c r="C9" s="103">
         <v>0</v>
       </c>
-      <c r="D9" s="104">
+      <c r="D9" s="103">
         <v>0.5</v>
       </c>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="105"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="104"/>
     </row>
     <row r="10" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="121"/>
+      <c r="C10" s="120"/>
     </row>
     <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="97"/>
-      <c r="B11" s="98" t="s">
+      <c r="A11" s="96"/>
+      <c r="B11" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="98">
+      <c r="C11" s="97">
         <v>0</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="97">
         <v>1</v>
       </c>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98">
+      <c r="E11" s="97"/>
+      <c r="F11" s="97">
         <v>45</v>
       </c>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="99"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="98"/>
     </row>
     <row r="12" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="100"/>
-      <c r="B12" s="101" t="s">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="121">
+      <c r="C12" s="120">
         <v>0</v>
       </c>
-      <c r="D12" s="121">
+      <c r="D12" s="120">
         <v>1</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101">
+      <c r="E12" s="100"/>
+      <c r="F12" s="100">
         <v>225</v>
       </c>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="102"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="101"/>
     </row>
     <row r="13" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103"/>
-      <c r="B13" s="104" t="s">
+      <c r="A13" s="102"/>
+      <c r="B13" s="103" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="104">
+      <c r="C13" s="103">
         <v>0</v>
       </c>
-      <c r="D13" s="104">
+      <c r="D13" s="103">
         <v>0.5</v>
       </c>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104">
+      <c r="E13" s="103"/>
+      <c r="F13" s="103">
         <v>45</v>
       </c>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="105"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="104"/>
     </row>
     <row r="14" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="112"/>
-      <c r="B15" s="98" t="s">
+      <c r="A15" s="111"/>
+      <c r="B15" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="98">
+      <c r="C15" s="97">
         <v>0</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="97">
         <v>1</v>
       </c>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98">
+      <c r="E15" s="97"/>
+      <c r="F15" s="97">
         <v>135</v>
       </c>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="99"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="98"/>
     </row>
     <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="113"/>
-      <c r="B16" s="101" t="s">
+      <c r="A16" s="112"/>
+      <c r="B16" s="100" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="121">
+      <c r="C16" s="120">
         <v>0</v>
       </c>
-      <c r="D16" s="121">
+      <c r="D16" s="120">
         <v>1</v>
       </c>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101">
+      <c r="E16" s="100"/>
+      <c r="F16" s="100">
         <v>315</v>
       </c>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="102"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="101"/>
     </row>
     <row r="17" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="114"/>
-      <c r="B17" s="104" t="s">
+      <c r="A17" s="113"/>
+      <c r="B17" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="104">
+      <c r="C17" s="103">
         <v>0</v>
       </c>
-      <c r="D17" s="104">
+      <c r="D17" s="103">
         <v>0.5</v>
       </c>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104">
+      <c r="E17" s="103"/>
+      <c r="F17" s="103">
         <v>135</v>
       </c>
-      <c r="G17" s="104"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="105"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="104"/>
     </row>
     <row r="18" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="115"/>
-      <c r="B19" s="98" t="s">
+      <c r="A19" s="114"/>
+      <c r="B19" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="98">
+      <c r="C19" s="97">
         <v>0</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="97">
         <v>1</v>
       </c>
-      <c r="E19" s="98" t="s">
+      <c r="E19" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="99"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="98"/>
     </row>
     <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="116"/>
-      <c r="B20" s="101" t="s">
+      <c r="A20" s="115"/>
+      <c r="B20" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="121">
+      <c r="C20" s="120">
         <v>0</v>
       </c>
-      <c r="D20" s="121">
+      <c r="D20" s="120">
         <v>1</v>
       </c>
-      <c r="E20" s="101" t="s">
+      <c r="E20" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101">
+      <c r="F20" s="100"/>
+      <c r="G20" s="100">
         <v>1</v>
       </c>
-      <c r="H20" s="101">
+      <c r="H20" s="100">
         <v>1</v>
       </c>
-      <c r="I20" s="101"/>
-      <c r="J20" s="102"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="101"/>
     </row>
     <row r="21" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="117"/>
-      <c r="B21" s="101" t="s">
+      <c r="A21" s="116"/>
+      <c r="B21" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="121">
+      <c r="C21" s="120">
         <v>0</v>
       </c>
-      <c r="D21" s="121">
+      <c r="D21" s="120">
         <v>1</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="101"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101"/>
-      <c r="I21" s="101">
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100">
         <v>1</v>
       </c>
-      <c r="J21" s="102">
+      <c r="J21" s="101">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="118"/>
-      <c r="B22" s="104" t="s">
+      <c r="A22" s="117"/>
+      <c r="B22" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="C22" s="104">
+      <c r="C22" s="103">
         <v>0</v>
       </c>
-      <c r="D22" s="104">
+      <c r="D22" s="103">
         <v>1</v>
       </c>
-      <c r="E22" s="104" t="s">
+      <c r="E22" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="F22" s="104"/>
-      <c r="G22" s="104">
+      <c r="F22" s="103"/>
+      <c r="G22" s="103">
         <v>1</v>
       </c>
-      <c r="H22" s="104">
+      <c r="H22" s="103">
         <v>1</v>
       </c>
-      <c r="I22" s="104">
+      <c r="I22" s="103">
         <v>1</v>
       </c>
-      <c r="J22" s="105">
+      <c r="J22" s="104">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="119"/>
-      <c r="B24" s="98" t="s">
+      <c r="A24" s="118"/>
+      <c r="B24" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="98">
+      <c r="C24" s="97">
         <v>0</v>
       </c>
-      <c r="D24" s="98">
+      <c r="D24" s="97">
         <v>1</v>
       </c>
-      <c r="E24" s="98" t="s">
+      <c r="E24" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98">
+      <c r="F24" s="97"/>
+      <c r="G24" s="97">
         <v>0.5</v>
       </c>
-      <c r="H24" s="98">
+      <c r="H24" s="97">
         <v>0.5</v>
       </c>
-      <c r="I24" s="98">
+      <c r="I24" s="97">
         <v>0.5</v>
       </c>
-      <c r="J24" s="99">
+      <c r="J24" s="98">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="120"/>
-      <c r="B25" s="104" t="s">
+      <c r="A25" s="119"/>
+      <c r="B25" s="103" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="104">
+      <c r="C25" s="103">
         <v>0</v>
       </c>
-      <c r="D25" s="104">
+      <c r="D25" s="103">
         <v>1</v>
       </c>
-      <c r="E25" s="104" t="s">
+      <c r="E25" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="F25" s="104"/>
-      <c r="G25" s="104">
+      <c r="F25" s="103"/>
+      <c r="G25" s="103">
         <v>0.5</v>
       </c>
-      <c r="H25" s="104">
+      <c r="H25" s="103">
         <v>0.5</v>
       </c>
-      <c r="I25" s="104">
+      <c r="I25" s="103">
         <v>0.5</v>
       </c>
-      <c r="J25" s="105">
+      <c r="J25" s="104">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>